<commit_message>
Updated Timesheet for Week 6
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C825AF0-47B9-42F2-98AE-D24A55872608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3884ED-1572-4951-80D7-23788565F187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="600" windowWidth="22980" windowHeight="12360" tabRatio="560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="26">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Got gitHub repository set up</t>
+  </si>
+  <si>
+    <t>Created more pages for the site</t>
   </si>
 </sst>
 </file>
@@ -736,7 +739,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +804,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +869,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +934,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +999,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -1061,7 +1064,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -1126,7 +1129,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1630,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1687,13 +1690,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43509</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>2.25</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>3.5</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,7 +1722,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -1767,7 +1787,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -1832,7 +1852,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1917,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>35.83</v>
+        <v>38.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Timesheet for week 7
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3884ED-1572-4951-80D7-23788565F187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D1DD0-2875-4DC4-8499-742FD7AA0789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="27">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Created more pages for the site</t>
+  </si>
+  <si>
+    <t>Worked on Admin Area Content</t>
   </si>
 </sst>
 </file>
@@ -739,7 +742,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +807,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +872,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +937,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +1002,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -1129,7 +1132,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -1496,7 +1499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A26" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1629,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1745,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1772,13 +1775,53 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43516</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43517</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1787,7 +1830,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1895,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +1960,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>38.08</v>
+        <v>41.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for week 8
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D1DD0-2875-4DC4-8499-742FD7AA0789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384DC32-AD92-426B-BB55-9DCFD34D43CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Worked on Admin Area Content</t>
+  </si>
+  <si>
+    <t>Created remaining pages</t>
+  </si>
+  <si>
+    <t>Worked on page content and CSS</t>
   </si>
 </sst>
 </file>
@@ -742,7 +748,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -807,7 +813,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -872,7 +878,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -937,7 +943,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -1002,7 +1008,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1073,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1138,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -1748,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1853,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1880,13 +1886,47 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43521</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43523</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>2.75</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1895,7 +1935,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>
@@ -1960,7 +2000,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>41.83</v>
+        <v>46.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added times to timesheet
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384DC32-AD92-426B-BB55-9DCFD34D43CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CBB4CD-0CE2-4D0C-A327-D0967EE2C3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="560" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="30">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Worked on page content and CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on CSS </t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -813,7 +816,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -878,7 +881,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +946,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -1008,7 +1011,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1076,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +1141,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1958,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1985,13 +1988,64 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43528</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43532</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43533</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2000,7 +2054,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>46.58</v>
+        <v>51.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated timesheet for this week
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB29DB0-0351-4C0C-9667-F566F046BBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B85F3F0-B0E3-43D4-9B8C-4663208F76F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="34">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Started Usability Testing and worked on CSS</t>
+  </si>
+  <si>
+    <t>Implemented some changes from accesability testing</t>
+  </si>
+  <si>
+    <t>Worked on Javascript</t>
   </si>
 </sst>
 </file>
@@ -715,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -831,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -858,13 +864,47 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43544</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43545</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -873,7 +913,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>58.33</v>
+        <v>62.08</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +978,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>58.33</v>
+        <v>62.08</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1043,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>58.33</v>
+        <v>62.08</v>
       </c>
     </row>
   </sheetData>
@@ -1068,7 +1108,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>58.33</v>
+        <v>62.08</v>
       </c>
     </row>
   </sheetData>
@@ -1133,7 +1173,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>58.33</v>
+        <v>62.08</v>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +1238,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>58.33</v>
+        <v>62.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added week 13 Info
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA7A6F-DFF6-47D2-89D6-D55704BCA035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF24EC-0296-4DB3-94BF-4E7342978776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Worked on checkout and return functions</t>
+  </si>
+  <si>
+    <t>Worked on Wish List feature</t>
+  </si>
+  <si>
+    <t>Finished Integrating Search Feature</t>
+  </si>
+  <si>
+    <t>Worked on Wish List and Search Feature</t>
   </si>
 </sst>
 </file>
@@ -942,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1041,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1068,13 +1077,64 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43560</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43565</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43567</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1083,7 +1143,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>65.83</v>
+        <v>72.08</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1208,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>65.83</v>
+        <v>72.08</v>
       </c>
     </row>
   </sheetData>
@@ -1213,7 +1273,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>65.83</v>
+        <v>72.08</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A11" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1278,7 +1338,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>65.83</v>
+        <v>72.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added timesheet information for week 14
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF24EC-0296-4DB3-94BF-4E7342978776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DD757A-7614-4FBC-9E1B-0DC19344793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="42">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Worked on Wish List and Search Feature</t>
+  </si>
+  <si>
+    <t>Implemented Captcha and started on reset password</t>
+  </si>
+  <si>
+    <t>Implementing usability test changes</t>
+  </si>
+  <si>
+    <t>Finished Reset Password Email functionality</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1166,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1193,13 +1202,64 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43572</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43573</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43575</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1208,7 +1268,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>72.08</v>
+        <v>79.83</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1333,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>72.08</v>
+        <v>79.83</v>
       </c>
     </row>
   </sheetData>
@@ -1338,7 +1398,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>72.08</v>
+        <v>79.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for final week
</commit_message>
<xml_diff>
--- a/mackey-sean-timesheet.xlsx
+++ b/mackey-sean-timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web289\gamingLibrarySite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFCFF81-3490-4E14-86A1-8FAA8B9C4B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3191DF1-D908-4386-A9D7-128A60292C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="0" windowWidth="22980" windowHeight="12360" tabRatio="560" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Started Cleaning up coding</t>
+  </si>
+  <si>
+    <t>4/31/2023</t>
+  </si>
+  <si>
+    <t>Cleaned up code and gathered everything to submit</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1403,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1423,13 +1429,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1438,7 +1461,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>79.83</v>
+        <v>84.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>